<commit_message>
started work on UI
</commit_message>
<xml_diff>
--- a/TestBook.xlsx
+++ b/TestBook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markn\Workspace\MaterializeExcelNew\MaterializeExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markn\Workspace\MaterializeExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73186F31-004E-49D9-9463-EDB20991877B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1B47A5-D155-4A37-B465-564507FE1E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11850" yWindow="4275" windowWidth="37035" windowHeight="15435" xr2:uid="{2CC1363C-DA3E-4E59-9C8E-4F96FE845EB2}"/>
+    <workbookView xWindow="7665" yWindow="3495" windowWidth="16785" windowHeight="13440" xr2:uid="{2CC1363C-DA3E-4E59-9C8E-4F96FE845EB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,28 +33,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -123,21 +101,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
-<volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <volType type="realTimeData">
-    <main first="rtdsrv_7f64a239d17648708c0d87a98af6428b">
-      <tp>
-        <v>6169</v>
-        <stp/>
-        <stp>6ec85333-3d6c-4644-a504-b4a406fd9ecb</stp>
-        <tr r="A2" s="1"/>
-      </tp>
-    </main>
-  </volType>
-</volTypes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -437,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B992668-698B-4517-9133-E02381D3FEDC}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -452,197 +415,9 @@
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:E12">_xll.MZ_TAIL(A1)</f>
-        <v>owner_id</v>
-      </c>
-      <c r="B2" t="str">
-        <v>owner_email</v>
-      </c>
-      <c r="C2" t="str">
-        <v>viewer_id</v>
-      </c>
-      <c r="D2" t="str">
-        <v>viewer_email</v>
-      </c>
-      <c r="E2" t="str">
-        <v>received_at</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>25</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Treva.Mock@facilisisuscipit.org</v>
-      </c>
-      <c r="C3">
-        <v>4768</v>
-      </c>
-      <c r="D3" t="str">
-        <v>Juli@induis.gov</v>
-      </c>
-      <c r="E3">
-        <v>1661534786</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>25</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Treva.Mock@facilisisuscipit.org</v>
-      </c>
-      <c r="C4">
-        <v>9560</v>
-      </c>
-      <c r="D4" t="str">
-        <v>Sammy@erostation.gov</v>
-      </c>
-      <c r="E4">
-        <v>1661534785</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>25</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Treva.Mock@facilisisuscipit.org</v>
-      </c>
-      <c r="C5">
-        <v>5383</v>
-      </c>
-      <c r="D5" t="str">
-        <v>Matilde@adfacilisis.com</v>
-      </c>
-      <c r="E5">
-        <v>1661534785</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
-        <v>25</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Treva.Mock@facilisisuscipit.org</v>
-      </c>
-      <c r="C6">
-        <v>2309</v>
-      </c>
-      <c r="D6" t="str">
-        <v>L.Hutchings@diamnislut.us</v>
-      </c>
-      <c r="E6">
-        <v>1661534793</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
-        <v>25</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Treva.Mock@facilisisuscipit.org</v>
-      </c>
-      <c r="C7">
-        <v>116</v>
-      </c>
-      <c r="D7" t="str">
-        <v>Marlin.Belt@odiodolore.net</v>
-      </c>
-      <c r="E7">
-        <v>1661534793</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8">
-        <v>25</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Treva.Mock@facilisisuscipit.org</v>
-      </c>
-      <c r="C8">
-        <v>4383</v>
-      </c>
-      <c r="D8" t="str">
-        <v>H.Ridenour@iustoetaccumsan.edu</v>
-      </c>
-      <c r="E8">
-        <v>1661534782</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9">
-        <v>25</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Treva.Mock@facilisisuscipit.org</v>
-      </c>
-      <c r="C9">
-        <v>5581</v>
-      </c>
-      <c r="D9" t="str">
-        <v>Enoch.Jacobsen@eufeugiatad.com</v>
-      </c>
-      <c r="E9">
-        <v>1661534797</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
-        <v>25</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Treva.Mock@facilisisuscipit.org</v>
-      </c>
-      <c r="C10">
-        <v>9254</v>
-      </c>
-      <c r="D10" t="str">
-        <v>Audrey.Carson@laoreetaccumsan.eu</v>
-      </c>
-      <c r="E10">
-        <v>1661534779</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11">
-        <v>25</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Treva.Mock@facilisisuscipit.org</v>
-      </c>
-      <c r="C11">
-        <v>9154</v>
-      </c>
-      <c r="D11" t="str">
-        <v>D.Oreilly@atcommodoconsequat.info</v>
-      </c>
-      <c r="E11">
-        <v>1661534789</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
-        <v>25</v>
-      </c>
-      <c r="B12" t="str">
-        <v>Treva.Mock@facilisisuscipit.org</v>
-      </c>
-      <c r="C12">
-        <v>7689</v>
-      </c>
-      <c r="D12" t="str">
-        <v>Noble@laoreetcommodoconsequat.info</v>
-      </c>
-      <c r="E12">
-        <v>1661534792</v>
       </c>
     </row>
   </sheetData>

</xml_diff>